<commit_message>
Agregar Casillas al xslx
</commit_message>
<xml_diff>
--- a/Sabana Tarifación Planes Cerrados.xlsx
+++ b/Sabana Tarifación Planes Cerrados.xlsx
@@ -3,21 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QV4097\Documents\vergara\Tarifacion2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC427FB7-957C-4A53-BB12-605DF0B9B76B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5DAAED-0C68-4607-95F9-9150F4AC962B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-4815" windowWidth="29040" windowHeight="15840" xr2:uid="{A2B13591-668B-9644-9949-56521285F75A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A2B13591-668B-9644-9949-56521285F75A}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan Cerrado 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="3" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
     <definedName name="tasas_ap">'[1]Primas - Controles'!#REF!</definedName>
@@ -25,10 +26,10 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19709" uniqueCount="184">
   <si>
     <t>Cant asegurados</t>
   </si>
@@ -144,6 +145,450 @@
   </si>
   <si>
     <t>Cuenta de ESTADO</t>
+  </si>
+  <si>
+    <t>TotalPrima</t>
+  </si>
+  <si>
+    <t>TotalPrimaMensual</t>
+  </si>
+  <si>
+    <t>nul</t>
+  </si>
+  <si>
+    <t>14381600,00</t>
+  </si>
+  <si>
+    <t>7190800,00</t>
+  </si>
+  <si>
+    <t>69031500,00</t>
+  </si>
+  <si>
+    <t>17257875,00</t>
+  </si>
+  <si>
+    <t>132754000,00</t>
+  </si>
+  <si>
+    <t>66377000,00</t>
+  </si>
+  <si>
+    <t>639185000,00</t>
+  </si>
+  <si>
+    <t>53265416,67</t>
+  </si>
+  <si>
+    <t>677990500,00</t>
+  </si>
+  <si>
+    <t>18478300,00</t>
+  </si>
+  <si>
+    <t>1539858,33</t>
+  </si>
+  <si>
+    <t>88695500,00</t>
+  </si>
+  <si>
+    <t>44347750,00</t>
+  </si>
+  <si>
+    <t>170568000,00</t>
+  </si>
+  <si>
+    <t>85284000,00</t>
+  </si>
+  <si>
+    <t>821260000,00</t>
+  </si>
+  <si>
+    <t>410630000,00</t>
+  </si>
+  <si>
+    <t>871112000,00</t>
+  </si>
+  <si>
+    <t>22176700,00</t>
+  </si>
+  <si>
+    <t>11088350,00</t>
+  </si>
+  <si>
+    <t>106447500,00</t>
+  </si>
+  <si>
+    <t>8870625,00</t>
+  </si>
+  <si>
+    <t>204708000,00</t>
+  </si>
+  <si>
+    <t>102354000,00</t>
+  </si>
+  <si>
+    <t>985630000,00</t>
+  </si>
+  <si>
+    <t>82135833,33</t>
+  </si>
+  <si>
+    <t>1045473000,00</t>
+  </si>
+  <si>
+    <t>261368250,00</t>
+  </si>
+  <si>
+    <t>26651200,00</t>
+  </si>
+  <si>
+    <t>13325600,00</t>
+  </si>
+  <si>
+    <t>127926000,00</t>
+  </si>
+  <si>
+    <t>10660500,00</t>
+  </si>
+  <si>
+    <t>246010000,00</t>
+  </si>
+  <si>
+    <t>20500833,33</t>
+  </si>
+  <si>
+    <t>1184500000,00</t>
+  </si>
+  <si>
+    <t>1256409000,00</t>
+  </si>
+  <si>
+    <t>20001400,00</t>
+  </si>
+  <si>
+    <t>1666783,33</t>
+  </si>
+  <si>
+    <t>96006500,00</t>
+  </si>
+  <si>
+    <t>8000541,67</t>
+  </si>
+  <si>
+    <t>184627000,00</t>
+  </si>
+  <si>
+    <t>15385583,33</t>
+  </si>
+  <si>
+    <t>888950000,00</t>
+  </si>
+  <si>
+    <t>222237500,00</t>
+  </si>
+  <si>
+    <t>942914500,00</t>
+  </si>
+  <si>
+    <t>235728625,00</t>
+  </si>
+  <si>
+    <t>25679500,00</t>
+  </si>
+  <si>
+    <t>6419875,00</t>
+  </si>
+  <si>
+    <t>123261500,00</t>
+  </si>
+  <si>
+    <t>61630750,00</t>
+  </si>
+  <si>
+    <t>237042000,00</t>
+  </si>
+  <si>
+    <t>59260500,00</t>
+  </si>
+  <si>
+    <t>1141315000,00</t>
+  </si>
+  <si>
+    <t>570657500,00</t>
+  </si>
+  <si>
+    <t>1210610500,00</t>
+  </si>
+  <si>
+    <t>30793800,00</t>
+  </si>
+  <si>
+    <t>15396900,00</t>
+  </si>
+  <si>
+    <t>147810500,00</t>
+  </si>
+  <si>
+    <t>36952625,00</t>
+  </si>
+  <si>
+    <t>284252000,00</t>
+  </si>
+  <si>
+    <t>1368625000,00</t>
+  </si>
+  <si>
+    <t>1451714000,00</t>
+  </si>
+  <si>
+    <t>725857000,00</t>
+  </si>
+  <si>
+    <t>36931900,00</t>
+  </si>
+  <si>
+    <t>9232975,00</t>
+  </si>
+  <si>
+    <t>177272500,00</t>
+  </si>
+  <si>
+    <t>88636250,00</t>
+  </si>
+  <si>
+    <t>340909000,00</t>
+  </si>
+  <si>
+    <t>85227250,00</t>
+  </si>
+  <si>
+    <t>1641415000,00</t>
+  </si>
+  <si>
+    <t>410353750,00</t>
+  </si>
+  <si>
+    <t>1741069000,00</t>
+  </si>
+  <si>
+    <t>870534500,00</t>
+  </si>
+  <si>
+    <t>28763300,00</t>
+  </si>
+  <si>
+    <t>7190825,00</t>
+  </si>
+  <si>
+    <t>138063500,00</t>
+  </si>
+  <si>
+    <t>69031750,00</t>
+  </si>
+  <si>
+    <t>265507000,00</t>
+  </si>
+  <si>
+    <t>1278370000,00</t>
+  </si>
+  <si>
+    <t>106530833,33</t>
+  </si>
+  <si>
+    <t>1355981000,00</t>
+  </si>
+  <si>
+    <t>112998416,67</t>
+  </si>
+  <si>
+    <t>36956400,00</t>
+  </si>
+  <si>
+    <t>9239100,00</t>
+  </si>
+  <si>
+    <t>177390500,00</t>
+  </si>
+  <si>
+    <t>341137000,00</t>
+  </si>
+  <si>
+    <t>85284250,00</t>
+  </si>
+  <si>
+    <t>1642505000,00</t>
+  </si>
+  <si>
+    <t>1742229500,00</t>
+  </si>
+  <si>
+    <t>435557375,00</t>
+  </si>
+  <si>
+    <t>44353100,00</t>
+  </si>
+  <si>
+    <t>11088275,00</t>
+  </si>
+  <si>
+    <t>212895500,00</t>
+  </si>
+  <si>
+    <t>53223875,00</t>
+  </si>
+  <si>
+    <t>409414000,00</t>
+  </si>
+  <si>
+    <t>34117833,33</t>
+  </si>
+  <si>
+    <t>1971255000,00</t>
+  </si>
+  <si>
+    <t>985627500,00</t>
+  </si>
+  <si>
+    <t>2090935000,00</t>
+  </si>
+  <si>
+    <t>522733750,00</t>
+  </si>
+  <si>
+    <t>53302400,00</t>
+  </si>
+  <si>
+    <t>255851500,00</t>
+  </si>
+  <si>
+    <t>63962875,00</t>
+  </si>
+  <si>
+    <t>492022000,00</t>
+  </si>
+  <si>
+    <t>123005500,00</t>
+  </si>
+  <si>
+    <t>2369000000,00</t>
+  </si>
+  <si>
+    <t>592250000,00</t>
+  </si>
+  <si>
+    <t>2512829000,00</t>
+  </si>
+  <si>
+    <t>628207250,00</t>
+  </si>
+  <si>
+    <t>34382900,00</t>
+  </si>
+  <si>
+    <t>17191450,00</t>
+  </si>
+  <si>
+    <t>165038000,00</t>
+  </si>
+  <si>
+    <t>317381000,00</t>
+  </si>
+  <si>
+    <t>1528130000,00</t>
+  </si>
+  <si>
+    <t>382032500,00</t>
+  </si>
+  <si>
+    <t>1620910500,00</t>
+  </si>
+  <si>
+    <t>810455250,00</t>
+  </si>
+  <si>
+    <t>44157800,00</t>
+  </si>
+  <si>
+    <t>11039450,00</t>
+  </si>
+  <si>
+    <t>211957000,00</t>
+  </si>
+  <si>
+    <t>105978500,00</t>
+  </si>
+  <si>
+    <t>407611000,00</t>
+  </si>
+  <si>
+    <t>101902750,00</t>
+  </si>
+  <si>
+    <t>1962570000,00</t>
+  </si>
+  <si>
+    <t>490642500,00</t>
+  </si>
+  <si>
+    <t>2081722500,00</t>
+  </si>
+  <si>
+    <t>173476875,00</t>
+  </si>
+  <si>
+    <t>52970600,00</t>
+  </si>
+  <si>
+    <t>254258500,00</t>
+  </si>
+  <si>
+    <t>127129250,00</t>
+  </si>
+  <si>
+    <t>488960000,00</t>
+  </si>
+  <si>
+    <t>40746666,67</t>
+  </si>
+  <si>
+    <t>2354245000,00</t>
+  </si>
+  <si>
+    <t>196187083,33</t>
+  </si>
+  <si>
+    <t>2497187000,00</t>
+  </si>
+  <si>
+    <t>1248593500,00</t>
+  </si>
+  <si>
+    <t>63583000,00</t>
+  </si>
+  <si>
+    <t>5298583,33</t>
+  </si>
+  <si>
+    <t>305198500,00</t>
+  </si>
+  <si>
+    <t>586920000,00</t>
+  </si>
+  <si>
+    <t>48910000,00</t>
+  </si>
+  <si>
+    <t>2825910000,00</t>
+  </si>
+  <si>
+    <t>235492500,00</t>
+  </si>
+  <si>
+    <t>2997483500,00</t>
+  </si>
+  <si>
+    <t>1498741750,00</t>
   </si>
 </sst>
 </file>
@@ -153,7 +598,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -193,14 +638,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -336,6 +780,34 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -369,6 +841,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-2373-4173-B45B-D159A260F041}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -384,6 +861,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-2373-4173-B45B-D159A260F041}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -1219,7 +1701,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="QV4097" refreshedDate="45049.892345949076" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="80" xr:uid="{95E5621E-30DC-4D29-A46C-706B7659811A}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="V1:V81" sheet="Plan Cerrado 1"/>
+    <worksheetSource ref="V1:V3" sheet="Plan Cerrado 1"/>
   </cacheSource>
   <cacheFields count="1">
     <cacheField name="ESTADO" numFmtId="0">
@@ -1483,7 +1965,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1A29EE32-02B7-4461-BC4E-445F73C8EDB4}" name="TablaDinámica1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1A29EE32-02B7-4461-BC4E-445F73C8EDB4}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
   <location ref="A1:B4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -1514,7 +1996,7 @@
   <dataFields count="1">
     <dataField name="Cuenta de ESTADO" fld="0" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="2">
+  <chartFormats count="4">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -1529,6 +2011,30 @@
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
@@ -1843,21 +2349,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D841E5DA-5C45-5145-97E1-44A8067B742F}">
-  <dimension ref="A1:V81"/>
+  <dimension ref="A1:X81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2:V81"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:X81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.44140625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="17.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="18.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="38.42578125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="19.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1924,8 +2431,14 @@
       <c r="V1" t="s">
         <v>30</v>
       </c>
+      <c r="W1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1992,8 +2505,14 @@
       <c r="V2" t="s">
         <v>31</v>
       </c>
+      <c r="W2" t="s">
+        <v>39</v>
+      </c>
+      <c r="X2" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -2060,8 +2579,14 @@
       <c r="V3" t="s">
         <v>31</v>
       </c>
+      <c r="W3" t="s">
+        <v>41</v>
+      </c>
+      <c r="X3" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -2128,8 +2653,14 @@
       <c r="V4" t="s">
         <v>31</v>
       </c>
+      <c r="W4" t="s">
+        <v>43</v>
+      </c>
+      <c r="X4" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -2196,8 +2727,14 @@
       <c r="V5" t="s">
         <v>31</v>
       </c>
+      <c r="W5" t="s">
+        <v>45</v>
+      </c>
+      <c r="X5" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -2264,8 +2801,14 @@
       <c r="V6" t="s">
         <v>31</v>
       </c>
+      <c r="W6" t="s">
+        <v>47</v>
+      </c>
+      <c r="X6" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -2332,8 +2875,14 @@
       <c r="V7" t="s">
         <v>32</v>
       </c>
+      <c r="W7" t="s">
+        <v>48</v>
+      </c>
+      <c r="X7" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -2400,8 +2949,14 @@
       <c r="V8" t="s">
         <v>32</v>
       </c>
+      <c r="W8" t="s">
+        <v>50</v>
+      </c>
+      <c r="X8" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -2468,8 +3023,14 @@
       <c r="V9" t="s">
         <v>32</v>
       </c>
+      <c r="W9" t="s">
+        <v>52</v>
+      </c>
+      <c r="X9" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -2536,8 +3097,14 @@
       <c r="V10" t="s">
         <v>32</v>
       </c>
+      <c r="W10" t="s">
+        <v>54</v>
+      </c>
+      <c r="X10" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -2604,8 +3171,14 @@
       <c r="V11" t="s">
         <v>32</v>
       </c>
+      <c r="W11" t="s">
+        <v>56</v>
+      </c>
+      <c r="X11" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -2672,8 +3245,14 @@
       <c r="V12" t="s">
         <v>32</v>
       </c>
+      <c r="W12" t="s">
+        <v>57</v>
+      </c>
+      <c r="X12" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -2740,8 +3319,14 @@
       <c r="V13" t="s">
         <v>32</v>
       </c>
+      <c r="W13" t="s">
+        <v>59</v>
+      </c>
+      <c r="X13" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2808,8 +3393,14 @@
       <c r="V14" t="s">
         <v>32</v>
       </c>
+      <c r="W14" t="s">
+        <v>61</v>
+      </c>
+      <c r="X14" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -2876,8 +3467,14 @@
       <c r="V15" t="s">
         <v>32</v>
       </c>
+      <c r="W15" t="s">
+        <v>63</v>
+      </c>
+      <c r="X15" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -2944,8 +3541,14 @@
       <c r="V16" t="s">
         <v>32</v>
       </c>
+      <c r="W16" t="s">
+        <v>65</v>
+      </c>
+      <c r="X16" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -3012,8 +3615,14 @@
       <c r="V17" t="s">
         <v>32</v>
       </c>
+      <c r="W17" t="s">
+        <v>67</v>
+      </c>
+      <c r="X17" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -3080,8 +3689,14 @@
       <c r="V18" t="s">
         <v>32</v>
       </c>
+      <c r="W18" t="s">
+        <v>69</v>
+      </c>
+      <c r="X18" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -3148,8 +3763,14 @@
       <c r="V19" t="s">
         <v>32</v>
       </c>
+      <c r="W19" t="s">
+        <v>71</v>
+      </c>
+      <c r="X19" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -3216,8 +3837,14 @@
       <c r="V20" t="s">
         <v>32</v>
       </c>
+      <c r="W20" t="s">
+        <v>73</v>
+      </c>
+      <c r="X20" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -3284,8 +3911,14 @@
       <c r="V21" t="s">
         <v>32</v>
       </c>
+      <c r="W21" t="s">
+        <v>74</v>
+      </c>
+      <c r="X21" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -3352,8 +3985,14 @@
       <c r="V22" t="s">
         <v>31</v>
       </c>
+      <c r="W22" t="s">
+        <v>75</v>
+      </c>
+      <c r="X22" t="s">
+        <v>76</v>
+      </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -3420,8 +4059,14 @@
       <c r="V23" t="s">
         <v>31</v>
       </c>
+      <c r="W23" t="s">
+        <v>77</v>
+      </c>
+      <c r="X23" t="s">
+        <v>78</v>
+      </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -3488,8 +4133,14 @@
       <c r="V24" t="s">
         <v>31</v>
       </c>
+      <c r="W24" t="s">
+        <v>79</v>
+      </c>
+      <c r="X24" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -3556,8 +4207,14 @@
       <c r="V25" t="s">
         <v>31</v>
       </c>
+      <c r="W25" t="s">
+        <v>81</v>
+      </c>
+      <c r="X25" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -3624,8 +4281,14 @@
       <c r="V26" t="s">
         <v>31</v>
       </c>
+      <c r="W26" t="s">
+        <v>83</v>
+      </c>
+      <c r="X26" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -3692,8 +4355,14 @@
       <c r="V27" t="s">
         <v>32</v>
       </c>
+      <c r="W27" t="s">
+        <v>85</v>
+      </c>
+      <c r="X27" t="s">
+        <v>86</v>
+      </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -3760,8 +4429,14 @@
       <c r="V28" t="s">
         <v>32</v>
       </c>
+      <c r="W28" t="s">
+        <v>87</v>
+      </c>
+      <c r="X28" t="s">
+        <v>88</v>
+      </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -3828,8 +4503,14 @@
       <c r="V29" t="s">
         <v>32</v>
       </c>
+      <c r="W29" t="s">
+        <v>89</v>
+      </c>
+      <c r="X29" t="s">
+        <v>90</v>
+      </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -3896,8 +4577,14 @@
       <c r="V30" t="s">
         <v>32</v>
       </c>
+      <c r="W30" t="s">
+        <v>91</v>
+      </c>
+      <c r="X30" t="s">
+        <v>92</v>
+      </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -3964,8 +4651,14 @@
       <c r="V31" t="s">
         <v>32</v>
       </c>
+      <c r="W31" t="s">
+        <v>93</v>
+      </c>
+      <c r="X31" t="s">
+        <v>93</v>
+      </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -4032,8 +4725,14 @@
       <c r="V32" t="s">
         <v>32</v>
       </c>
+      <c r="W32" t="s">
+        <v>94</v>
+      </c>
+      <c r="X32" t="s">
+        <v>95</v>
+      </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -4100,8 +4799,14 @@
       <c r="V33" t="s">
         <v>32</v>
       </c>
+      <c r="W33" t="s">
+        <v>96</v>
+      </c>
+      <c r="X33" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>24</v>
       </c>
@@ -4168,8 +4873,14 @@
       <c r="V34" t="s">
         <v>32</v>
       </c>
+      <c r="W34" t="s">
+        <v>98</v>
+      </c>
+      <c r="X34" t="s">
+        <v>98</v>
+      </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>24</v>
       </c>
@@ -4236,8 +4947,14 @@
       <c r="V35" t="s">
         <v>32</v>
       </c>
+      <c r="W35" t="s">
+        <v>99</v>
+      </c>
+      <c r="X35" t="s">
+        <v>99</v>
+      </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>24</v>
       </c>
@@ -4304,8 +5021,14 @@
       <c r="V36" t="s">
         <v>32</v>
       </c>
+      <c r="W36" t="s">
+        <v>100</v>
+      </c>
+      <c r="X36" t="s">
+        <v>101</v>
+      </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>24</v>
       </c>
@@ -4372,8 +5095,14 @@
       <c r="V37" t="s">
         <v>32</v>
       </c>
+      <c r="W37" t="s">
+        <v>102</v>
+      </c>
+      <c r="X37" t="s">
+        <v>103</v>
+      </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -4440,8 +5169,14 @@
       <c r="V38" t="s">
         <v>32</v>
       </c>
+      <c r="W38" t="s">
+        <v>104</v>
+      </c>
+      <c r="X38" t="s">
+        <v>105</v>
+      </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>24</v>
       </c>
@@ -4508,8 +5243,14 @@
       <c r="V39" t="s">
         <v>32</v>
       </c>
+      <c r="W39" t="s">
+        <v>106</v>
+      </c>
+      <c r="X39" t="s">
+        <v>107</v>
+      </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>24</v>
       </c>
@@ -4576,8 +5317,14 @@
       <c r="V40" t="s">
         <v>32</v>
       </c>
+      <c r="W40" t="s">
+        <v>108</v>
+      </c>
+      <c r="X40" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>24</v>
       </c>
@@ -4644,8 +5391,14 @@
       <c r="V41" t="s">
         <v>32</v>
       </c>
+      <c r="W41" t="s">
+        <v>110</v>
+      </c>
+      <c r="X41" t="s">
+        <v>111</v>
+      </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>24</v>
       </c>
@@ -4712,8 +5465,14 @@
       <c r="V42" t="s">
         <v>31</v>
       </c>
+      <c r="W42" t="s">
+        <v>112</v>
+      </c>
+      <c r="X42" t="s">
+        <v>113</v>
+      </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>24</v>
       </c>
@@ -4780,8 +5539,14 @@
       <c r="V43" t="s">
         <v>31</v>
       </c>
+      <c r="W43" t="s">
+        <v>114</v>
+      </c>
+      <c r="X43" t="s">
+        <v>115</v>
+      </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>24</v>
       </c>
@@ -4848,8 +5613,14 @@
       <c r="V44" t="s">
         <v>31</v>
       </c>
+      <c r="W44" t="s">
+        <v>116</v>
+      </c>
+      <c r="X44" t="s">
+        <v>116</v>
+      </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>24</v>
       </c>
@@ -4916,8 +5687,14 @@
       <c r="V45" t="s">
         <v>31</v>
       </c>
+      <c r="W45" t="s">
+        <v>117</v>
+      </c>
+      <c r="X45" t="s">
+        <v>118</v>
+      </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>24</v>
       </c>
@@ -4984,8 +5761,14 @@
       <c r="V46" t="s">
         <v>31</v>
       </c>
+      <c r="W46" t="s">
+        <v>119</v>
+      </c>
+      <c r="X46" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>24</v>
       </c>
@@ -5052,8 +5835,14 @@
       <c r="V47" t="s">
         <v>32</v>
       </c>
+      <c r="W47" t="s">
+        <v>121</v>
+      </c>
+      <c r="X47" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>24</v>
       </c>
@@ -5120,8 +5909,14 @@
       <c r="V48" t="s">
         <v>32</v>
       </c>
+      <c r="W48" t="s">
+        <v>123</v>
+      </c>
+      <c r="X48" t="s">
+        <v>123</v>
+      </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>24</v>
       </c>
@@ -5188,8 +5983,14 @@
       <c r="V49" t="s">
         <v>32</v>
       </c>
+      <c r="W49" t="s">
+        <v>124</v>
+      </c>
+      <c r="X49" t="s">
+        <v>125</v>
+      </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>24</v>
       </c>
@@ -5256,8 +6057,14 @@
       <c r="V50" t="s">
         <v>32</v>
       </c>
+      <c r="W50" t="s">
+        <v>126</v>
+      </c>
+      <c r="X50" t="s">
+        <v>126</v>
+      </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>24</v>
       </c>
@@ -5324,8 +6131,14 @@
       <c r="V51" t="s">
         <v>32</v>
       </c>
+      <c r="W51" t="s">
+        <v>127</v>
+      </c>
+      <c r="X51" t="s">
+        <v>128</v>
+      </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>24</v>
       </c>
@@ -5392,8 +6205,14 @@
       <c r="V52" t="s">
         <v>32</v>
       </c>
+      <c r="W52" t="s">
+        <v>129</v>
+      </c>
+      <c r="X52" t="s">
+        <v>130</v>
+      </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>24</v>
       </c>
@@ -5460,8 +6279,14 @@
       <c r="V53" t="s">
         <v>32</v>
       </c>
+      <c r="W53" t="s">
+        <v>131</v>
+      </c>
+      <c r="X53" t="s">
+        <v>132</v>
+      </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>24</v>
       </c>
@@ -5528,8 +6353,14 @@
       <c r="V54" t="s">
         <v>32</v>
       </c>
+      <c r="W54" t="s">
+        <v>133</v>
+      </c>
+      <c r="X54" t="s">
+        <v>134</v>
+      </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>24</v>
       </c>
@@ -5596,8 +6427,14 @@
       <c r="V55" t="s">
         <v>32</v>
       </c>
+      <c r="W55" t="s">
+        <v>135</v>
+      </c>
+      <c r="X55" t="s">
+        <v>136</v>
+      </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>24</v>
       </c>
@@ -5664,8 +6501,14 @@
       <c r="V56" t="s">
         <v>32</v>
       </c>
+      <c r="W56" t="s">
+        <v>137</v>
+      </c>
+      <c r="X56" t="s">
+        <v>138</v>
+      </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>24</v>
       </c>
@@ -5732,8 +6575,14 @@
       <c r="V57" t="s">
         <v>32</v>
       </c>
+      <c r="W57" t="s">
+        <v>139</v>
+      </c>
+      <c r="X57" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>24</v>
       </c>
@@ -5800,8 +6649,14 @@
       <c r="V58" t="s">
         <v>32</v>
       </c>
+      <c r="W58" t="s">
+        <v>140</v>
+      </c>
+      <c r="X58" t="s">
+        <v>141</v>
+      </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>24</v>
       </c>
@@ -5868,8 +6723,14 @@
       <c r="V59" t="s">
         <v>32</v>
       </c>
+      <c r="W59" t="s">
+        <v>142</v>
+      </c>
+      <c r="X59" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>24</v>
       </c>
@@ -5936,8 +6797,14 @@
       <c r="V60" t="s">
         <v>32</v>
       </c>
+      <c r="W60" t="s">
+        <v>144</v>
+      </c>
+      <c r="X60" t="s">
+        <v>145</v>
+      </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>24</v>
       </c>
@@ -6004,8 +6871,14 @@
       <c r="V61" t="s">
         <v>32</v>
       </c>
+      <c r="W61" t="s">
+        <v>146</v>
+      </c>
+      <c r="X61" t="s">
+        <v>147</v>
+      </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>24</v>
       </c>
@@ -6072,8 +6945,14 @@
       <c r="V62" t="s">
         <v>32</v>
       </c>
+      <c r="W62" t="s">
+        <v>148</v>
+      </c>
+      <c r="X62" t="s">
+        <v>149</v>
+      </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>24</v>
       </c>
@@ -6140,8 +7019,14 @@
       <c r="V63" t="s">
         <v>32</v>
       </c>
+      <c r="W63" t="s">
+        <v>150</v>
+      </c>
+      <c r="X63" t="s">
+        <v>150</v>
+      </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>24</v>
       </c>
@@ -6208,8 +7093,14 @@
       <c r="V64" t="s">
         <v>32</v>
       </c>
+      <c r="W64" t="s">
+        <v>151</v>
+      </c>
+      <c r="X64" t="s">
+        <v>151</v>
+      </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>24</v>
       </c>
@@ -6276,8 +7167,14 @@
       <c r="V65" t="s">
         <v>32</v>
       </c>
+      <c r="W65" t="s">
+        <v>152</v>
+      </c>
+      <c r="X65" t="s">
+        <v>153</v>
+      </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>24</v>
       </c>
@@ -6344,8 +7241,14 @@
       <c r="V66" t="s">
         <v>32</v>
       </c>
+      <c r="W66" t="s">
+        <v>154</v>
+      </c>
+      <c r="X66" t="s">
+        <v>155</v>
+      </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>24</v>
       </c>
@@ -6412,8 +7315,14 @@
       <c r="V67" t="s">
         <v>32</v>
       </c>
+      <c r="W67" t="s">
+        <v>156</v>
+      </c>
+      <c r="X67" t="s">
+        <v>157</v>
+      </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>24</v>
       </c>
@@ -6480,8 +7389,14 @@
       <c r="V68" t="s">
         <v>32</v>
       </c>
+      <c r="W68" t="s">
+        <v>158</v>
+      </c>
+      <c r="X68" t="s">
+        <v>159</v>
+      </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>24</v>
       </c>
@@ -6548,8 +7463,14 @@
       <c r="V69" t="s">
         <v>32</v>
       </c>
+      <c r="W69" t="s">
+        <v>160</v>
+      </c>
+      <c r="X69" t="s">
+        <v>161</v>
+      </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>24</v>
       </c>
@@ -6616,8 +7537,14 @@
       <c r="V70" t="s">
         <v>32</v>
       </c>
+      <c r="W70" t="s">
+        <v>162</v>
+      </c>
+      <c r="X70" t="s">
+        <v>163</v>
+      </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>24</v>
       </c>
@@ -6684,8 +7611,14 @@
       <c r="V71" t="s">
         <v>32</v>
       </c>
+      <c r="W71" t="s">
+        <v>164</v>
+      </c>
+      <c r="X71" t="s">
+        <v>165</v>
+      </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>24</v>
       </c>
@@ -6752,8 +7685,14 @@
       <c r="V72" t="s">
         <v>32</v>
       </c>
+      <c r="W72" t="s">
+        <v>166</v>
+      </c>
+      <c r="X72" t="s">
+        <v>166</v>
+      </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>24</v>
       </c>
@@ -6820,8 +7759,14 @@
       <c r="V73" t="s">
         <v>32</v>
       </c>
+      <c r="W73" t="s">
+        <v>167</v>
+      </c>
+      <c r="X73" t="s">
+        <v>168</v>
+      </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>24</v>
       </c>
@@ -6888,8 +7833,14 @@
       <c r="V74" t="s">
         <v>32</v>
       </c>
+      <c r="W74" t="s">
+        <v>169</v>
+      </c>
+      <c r="X74" t="s">
+        <v>170</v>
+      </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>24</v>
       </c>
@@ -6956,8 +7907,14 @@
       <c r="V75" t="s">
         <v>32</v>
       </c>
+      <c r="W75" t="s">
+        <v>171</v>
+      </c>
+      <c r="X75" t="s">
+        <v>172</v>
+      </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>24</v>
       </c>
@@ -7024,8 +7981,14 @@
       <c r="V76" t="s">
         <v>32</v>
       </c>
+      <c r="W76" t="s">
+        <v>173</v>
+      </c>
+      <c r="X76" t="s">
+        <v>174</v>
+      </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>24</v>
       </c>
@@ -7092,8 +8055,14 @@
       <c r="V77" t="s">
         <v>32</v>
       </c>
+      <c r="W77" t="s">
+        <v>175</v>
+      </c>
+      <c r="X77" t="s">
+        <v>176</v>
+      </c>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>24</v>
       </c>
@@ -7160,8 +8129,14 @@
       <c r="V78" t="s">
         <v>32</v>
       </c>
+      <c r="W78" t="s">
+        <v>177</v>
+      </c>
+      <c r="X78" t="s">
+        <v>177</v>
+      </c>
     </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>24</v>
       </c>
@@ -7228,8 +8203,14 @@
       <c r="V79" t="s">
         <v>32</v>
       </c>
+      <c r="W79" t="s">
+        <v>178</v>
+      </c>
+      <c r="X79" t="s">
+        <v>179</v>
+      </c>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>24</v>
       </c>
@@ -7296,8 +8277,14 @@
       <c r="V80" t="s">
         <v>32</v>
       </c>
+      <c r="W80" t="s">
+        <v>180</v>
+      </c>
+      <c r="X80" t="s">
+        <v>181</v>
+      </c>
     </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>24</v>
       </c>
@@ -7363,6 +8350,12 @@
       </c>
       <c r="V81" t="s">
         <v>32</v>
+      </c>
+      <c r="W81" t="s">
+        <v>182</v>
+      </c>
+      <c r="X81" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -7372,6 +8365,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A2E590-D9DC-47AF-8CF1-DC4E25CE6AB9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:X78"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2577A8A-3111-4F3F-85FF-ACD557F1E2A3}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -7379,12 +8386,12 @@
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -7392,27 +8399,27 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4">
         <v>80</v>
       </c>
     </row>
@@ -7423,12 +8430,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3aec2603-24a0-491a-809b-d6c7badc813e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c8936e00-c3ac-4c42-aa24-65d953c54a25" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7649,20 +8658,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3aec2603-24a0-491a-809b-d6c7badc813e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c8936e00-c3ac-4c42-aa24-65d953c54a25" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAADA5A0-3EE0-4B4B-B2C7-185EA28905C7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61ED9210-5C27-476E-BFBE-45057404014E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3aec2603-24a0-491a-809b-d6c7badc813e"/>
+    <ds:schemaRef ds:uri="c8936e00-c3ac-4c42-aa24-65d953c54a25"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7687,12 +8697,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61ED9210-5C27-476E-BFBE-45057404014E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAADA5A0-3EE0-4B4B-B2C7-185EA28905C7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3aec2603-24a0-491a-809b-d6c7badc813e"/>
-    <ds:schemaRef ds:uri="c8936e00-c3ac-4c42-aa24-65d953c54a25"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>